<commit_message>
improved user-data persistence and reloading after SE run
</commit_message>
<xml_diff>
--- a/data/TCSDB/user_data.xlsx
+++ b/data/TCSDB/user_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3667,6 +3667,804 @@
         </is>
       </c>
     </row>
+    <row r="88">
+      <c r="A88">
+        <v>1519400664</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Boise </t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1000 </t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_10:44:24_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>1519403232</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Manassas </t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_11:27:12_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>1519404127</v>
+      </c>
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 997 </t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_11:42:07_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>1519404349</v>
+      </c>
+      <c r="B91">
+        <v>4</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_11:45:49_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>1519411962</v>
+      </c>
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Coronation_Drive_Office_Park </t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_13:52:42_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>1519411978</v>
+      </c>
+      <c r="B93">
+        <v>4</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Coronation_Drive_Office_Park </t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_13:52:58_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>1519412355</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Macquarie_Centre </t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_13:59:15_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>1519412485</v>
+      </c>
+      <c r="B95">
+        <v>4</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Macquarie_Centre </t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 100 </t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_14:01:25_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>1519412536</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Macquarie_Centre </t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_14:02:16_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>1519412681</v>
+      </c>
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Macquarie_Centre </t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 998 </t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_14:04:41_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>1519412850</v>
+      </c>
+      <c r="B98">
+        <v>4</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Macquarie_Centre </t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_14:07:30_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>1519412851</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Macquarie_Centre </t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_14:07:31_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>1519412868</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AMP_Building </t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 100 </t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fri_Feb_23_14:07:48_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>1519577983</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AMP_Building </t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 100 </t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, Shipping, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_11:59:43_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>1519585936</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, Inventory Management, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_14:12:16_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>1519585988</v>
+      </c>
+      <c r="B103">
+        <v>4</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D, HR </t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_14:13:08_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>1519588508</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  </t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_14:55:08_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>1519588688</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  </t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_14:58:08_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>1519588701</v>
+      </c>
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  </t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_14:58:21_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>1519589302</v>
+      </c>
+      <c r="B107">
+        <v>4</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Indooroopilly_Shopping_Centre </t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, Shipping, Inventory Management </t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sun_Feb_25_15:08:22_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>1519655158</v>
+      </c>
+      <c r="B108">
+        <v>4</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pacific_Fair </t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, Shipping, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_09:25:58_EST_2018</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed parsing bug in /data/TCSDB/script_apply_userdata4SE
</commit_message>
<xml_diff>
--- a/data/TCSDB/user_data.xlsx
+++ b/data/TCSDB/user_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4465,6 +4465,310 @@
         </is>
       </c>
     </row>
+    <row r="109">
+      <c r="A109">
+        <v>1519661118</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1000 </t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_11:05:18_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>1519661136</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1000 </t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_11:05:36_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>1519664173</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 100 </t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_11:56:13_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>1519664511</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_Hqs </t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 999 </t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_12:01:51_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>1519664549</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1000 </t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_12:02:29_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114">
+        <v>1519664962</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10000 </t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_12:09:22_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>1519667496</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_12:51:36_EST_2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>1519667630</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Singapore_300mm_NAND </t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 250 </t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9999 </t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mon_Feb_26_12:53:50_EST_2018</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added HP printer suppliers
</commit_message>
<xml_diff>
--- a/data/TCSDB/user_data.xlsx
+++ b/data/TCSDB/user_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H163"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,7 +401,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -433,13 +433,13 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -471,13 +471,13 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -509,13 +509,13 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -547,13 +547,13 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -585,13 +585,13 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -623,13 +623,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -661,13 +661,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -699,13 +699,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -737,13 +737,13 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -775,13 +775,13 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -813,13 +813,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -851,13 +851,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -889,13 +889,13 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -927,13 +927,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -965,13 +965,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1003,13 +1003,13 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1041,13 +1041,13 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1079,13 +1079,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1117,13 +1117,13 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1155,13 +1155,13 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1193,13 +1193,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1231,13 +1231,13 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1269,13 +1269,13 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1307,13 +1307,13 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1345,13 +1345,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1383,13 +1383,13 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1421,13 +1421,13 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1459,13 +1459,13 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1497,13 +1497,13 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1535,13 +1535,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -1573,13 +1573,13 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -1611,13 +1611,13 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1649,13 +1649,13 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -1687,13 +1687,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -1725,13 +1725,13 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -1763,13 +1763,13 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -1801,13 +1801,13 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -1839,13 +1839,13 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1877,13 +1877,13 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -1915,13 +1915,13 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1953,13 +1953,13 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -1991,13 +1991,13 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -2029,13 +2029,13 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -2067,13 +2067,13 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2105,20 +2105,20 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Indooroopilly_Shopping_Centre</t>
+          <t>SUP_Celestica_Malaysia</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2143,20 +2143,20 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Pacific_Fair</t>
+          <t>SUP_Flex_Brazil</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2181,20 +2181,20 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Stanley_Plaza</t>
+          <t>SUP_Flex_Malaysia</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2219,20 +2219,20 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Coronation_Drive_Office_Park</t>
+          <t>SUP_Jabil_Circuit_NL</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2257,20 +2257,20 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Macquarie_Centre</t>
+          <t>SUP_Venture_Malaysia</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2295,20 +2295,20 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B52">
         <v>4</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>AMP_Building</t>
+          <t>Indooroopilly_Shopping_Centre</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2333,20 +2333,20 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B53">
         <v>4</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>NAB_Headquarters</t>
+          <t>Pacific_Fair</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2371,20 +2371,20 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B54">
         <v>4</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Malvern_Central</t>
+          <t>Stanley_Plaza</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2409,20 +2409,20 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B55">
         <v>4</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Exchange_Tower</t>
+          <t>Coronation_Drive_Office_Park</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2447,20 +2447,20 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Garden_City</t>
+          <t>Macquarie_Centre</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2485,20 +2485,20 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B57">
         <v>4</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>The_Palms_NZ</t>
+          <t>AMP_Building</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2523,20 +2523,20 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Gridley_IL</t>
+          <t>NAB_Headquarters</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2561,20 +2561,20 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Blue_Earth_MN</t>
+          <t>Malvern_Central</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2599,20 +2599,20 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Bakersfield_CA</t>
+          <t>Exchange_Tower</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2637,20 +2637,20 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Foley_MN</t>
+          <t>Garden_City</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2675,20 +2675,20 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Mobile_AL_USA</t>
+          <t>The_Palms_NZ</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2713,20 +2713,20 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Columbus_MS_USA</t>
+          <t>Gridley_IL</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2751,20 +2751,20 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Grand_Prairie_TX_USA</t>
+          <t>Blue_Earth_MN</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2789,20 +2789,20 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Atlanta_GA_USA</t>
+          <t>Bakersfield_CA</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2827,20 +2827,20 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Miami_FL_USA</t>
+          <t>Foley_MN</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2865,20 +2865,20 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B67">
         <v>6</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Ashburn_VA_USA</t>
+          <t>Mobile_AL_USA</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2903,20 +2903,20 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B68">
         <v>6</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Hamburg_Germany</t>
+          <t>Columbus_MS_USA</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2941,20 +2941,20 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B69">
         <v>6</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Tianjin_China</t>
+          <t>Grand_Prairie_TX_USA</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2979,20 +2979,20 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B70">
         <v>6</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Toulouse_France</t>
+          <t>Atlanta_GA_USA</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3017,20 +3017,20 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B71">
         <v>6</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Queretaro_Mexico</t>
+          <t>Miami_FL_USA</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3055,20 +3055,20 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B72">
         <v>6</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Itajuba_Minas_Gerais_Brazil</t>
+          <t>Ashburn_VA_USA</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3093,20 +3093,20 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B73">
         <v>6</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Sao_Paulo_Brazil</t>
+          <t>Hamburg_Germany</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3131,20 +3131,20 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B74">
         <v>6</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Rio_de_Janeiro_Brazil</t>
+          <t>Tianjin_China</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3169,20 +3169,20 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B75">
         <v>6</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Brasilia_Brazil</t>
+          <t>Toulouse_France</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3207,20 +3207,20 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B76">
         <v>6</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Broughton_UK</t>
+          <t>Queretaro_Mexico</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3245,20 +3245,20 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B77">
         <v>6</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Bristol_UK</t>
+          <t>Itajuba_Minas_Gerais_Brazil</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3283,20 +3283,20 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B78">
         <v>6</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Stade_Germany</t>
+          <t>Sao_Paulo_Brazil</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3321,20 +3321,20 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B79">
         <v>6</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Bremen_Germany</t>
+          <t>Rio_de_Janeiro_Brazil</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3359,20 +3359,20 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B80">
         <v>6</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Donauworth_Germany</t>
+          <t>Brasilia_Brazil</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3397,20 +3397,20 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B81">
         <v>6</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Nantes_France</t>
+          <t>Broughton_UK</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3435,20 +3435,20 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B82">
         <v>6</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Marignane_France</t>
+          <t>Bristol_UK</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3473,20 +3473,20 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B83">
         <v>6</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Madrid_Spain</t>
+          <t>Stade_Germany</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3511,20 +3511,20 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B84">
         <v>6</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Sevilla_Spain</t>
+          <t>Bremen_Germany</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3549,20 +3549,20 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B85">
         <v>6</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Casablanca_Morocco</t>
+          <t>Donauworth_Germany</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3587,20 +3587,20 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B86">
         <v>6</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Blenheim_New_Zealand</t>
+          <t>Nantes_France</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3625,20 +3625,20 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B87">
         <v>6</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Brisbane_Australia</t>
+          <t>Marignane_France</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3663,20 +3663,20 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B88">
         <v>6</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Riyadh_Saudi_Arabia</t>
+          <t>Madrid_Spain</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3701,20 +3701,20 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B89">
         <v>6</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Jubail_Saudi_Arabia</t>
+          <t>Sevilla_Spain</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3739,20 +3739,20 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B90">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Campo_Grande_Brazil</t>
+          <t>Casablanca_Morocco</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3777,20 +3777,20 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B91">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Belo_Horizonte_Brazil</t>
+          <t>Blenheim_New_Zealand</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3815,20 +3815,20 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Porto_Real_Brazil</t>
+          <t>Brisbane_Australia</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -3853,20 +3853,20 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B93">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Mogi_das_Cruzes_Brazil</t>
+          <t>Riyadh_Saudi_Arabia</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3891,20 +3891,20 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B94">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Jundiai_Brazil</t>
+          <t>Jubail_Saudi_Arabia</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3929,20 +3929,20 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B95">
         <v>7</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Sao_Paulo_Brazil</t>
+          <t>Campo_Grande_Brazil</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3967,20 +3967,20 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B96">
         <v>7</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Curitiba_Brazil</t>
+          <t>Belo_Horizonte_Brazil</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -4005,20 +4005,20 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B97">
         <v>7</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Maringa_Brazil</t>
+          <t>Porto_Real_Brazil</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -4043,20 +4043,20 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B98">
         <v>7</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Marilia_Brazil</t>
+          <t>Mogi_das_Cruzes_Brazil</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -4081,20 +4081,20 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B99">
         <v>7</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Bauru_Brazil</t>
+          <t>Jundiai_Brazil</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -4119,20 +4119,20 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B100">
         <v>7</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>San_Cristobal_de_las_Casas_Mexico</t>
+          <t>Sao_Paulo_Brazil</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4157,20 +4157,20 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B101">
         <v>7</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Tabasco_Mexico</t>
+          <t>Curitiba_Brazil</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -4195,20 +4195,20 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B102">
         <v>7</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Coatepec_Mexico</t>
+          <t>Maringa_Brazil</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4233,20 +4233,20 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B103">
         <v>7</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Poza_Rica_Mexico</t>
+          <t>Marilia_Brazil</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -4271,20 +4271,20 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B104">
         <v>7</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Apizaco_Mexico</t>
+          <t>Bauru_Brazil</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -4309,20 +4309,20 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B105">
         <v>7</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Leon_Mexico</t>
+          <t>San_Cristobal_de_las_Casas_Mexico</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4347,20 +4347,20 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B106">
         <v>7</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Santiago_deA_Queretaro_Mexico</t>
+          <t>Tabasco_Mexico</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4385,20 +4385,20 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B107">
         <v>7</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Zinacantepec_Mexico</t>
+          <t>Coatepec_Mexico</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4423,20 +4423,20 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B108">
         <v>7</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Pinotepa_Nacional_Mexico</t>
+          <t>Poza_Rica_Mexico</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4461,20 +4461,20 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B109">
         <v>7</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Cuernavaca_Mexico</t>
+          <t>Apizaco_Mexico</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4499,20 +4499,20 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B110">
         <v>7</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Los_Reyes_Acaquilpan_Mexico</t>
+          <t>Leon_Mexico</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -4537,20 +4537,20 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B111">
         <v>7</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Cuautitlan_Izcalli_Mexico</t>
+          <t>Santiago_deA_Queretaro_Mexico</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -4575,20 +4575,20 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B112">
         <v>7</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Tepotzotlan_Mexico</t>
+          <t>Zinacantepec_Mexico</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -4613,20 +4613,20 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B113">
         <v>7</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Altamira_Mexico</t>
+          <t>Pinotepa_Nacional_Mexico</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -4651,20 +4651,20 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B114">
         <v>7</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Apizaco_Mexico</t>
+          <t>Cuernavaca_Mexico</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -4689,20 +4689,20 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B115">
         <v>7</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Morelia_Mexico</t>
+          <t>Los_Reyes_Acaquilpan_Mexico</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -4727,20 +4727,20 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B116">
         <v>7</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Cuajimalpa_de_Morelos_Mexico</t>
+          <t>Cuautitlan_Izcalli_Mexico</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -4765,20 +4765,20 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B117">
         <v>7</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Toluca_Mexico</t>
+          <t>Tepotzotlan_Mexico</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -4803,20 +4803,20 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B118">
         <v>7</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Tocancipa_Colombia</t>
+          <t>Altamira_Mexico</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -4841,20 +4841,20 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B119">
         <v>7</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Manantial_Colombia</t>
+          <t>Morelia_Mexico</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4879,20 +4879,20 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B120">
         <v>7</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Barranquilla_Colombia</t>
+          <t>Cuajimalpa_de_Morelos_Mexico</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4917,20 +4917,20 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B121">
         <v>7</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Bucaramanga_Colombia</t>
+          <t>Toluca_Mexico</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4955,20 +4955,20 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B122">
         <v>7</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Medellin_Colombia</t>
+          <t>Tocancipa_Colombia</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4993,20 +4993,20 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B123">
         <v>7</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Santiago_de_Cali_Colombia</t>
+          <t>Manantial_Colombia</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -5031,20 +5031,20 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B124">
         <v>7</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Bogota_Colombia</t>
+          <t>Barranquilla_Colombia</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -5069,20 +5069,20 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B125">
         <v>7</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Ilocos_Philippines</t>
+          <t>Bucaramanga_Colombia</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -5107,20 +5107,20 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B126">
         <v>7</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Ilagan_Philippines</t>
+          <t>Medellin_Colombia</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -5145,20 +5145,20 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B127">
         <v>7</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>San_Fernando_Philippines</t>
+          <t>Santiago_de_Cali_Colombia</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -5183,20 +5183,20 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B128">
         <v>7</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Meycauayan_Philippines</t>
+          <t>Bogota_Colombia</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -5221,20 +5221,20 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B129">
         <v>7</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Naga_Philippines</t>
+          <t>Ilocos_Philippines</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -5259,20 +5259,20 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B130">
         <v>7</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Tacloban_Philippines</t>
+          <t>Ilagan_Philippines</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -5297,20 +5297,20 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B131">
         <v>7</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Mandaue_Philippines</t>
+          <t>San_Fernando_Philippines</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -5335,20 +5335,20 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B132">
         <v>7</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Bacolod_Philippines</t>
+          <t>Meycauayan_Philippines</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -5373,20 +5373,20 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B133">
         <v>7</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Iloilo_Philippines</t>
+          <t>Naga_Philippines</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -5411,20 +5411,20 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B134">
         <v>7</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Tagbilaran_Philippines</t>
+          <t>Tacloban_Philippines</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -5449,20 +5449,20 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B135">
         <v>7</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Misasmis_Oriental_Philippines</t>
+          <t>Mandaue_Philippines</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -5487,20 +5487,20 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B136">
         <v>7</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Davao_Philippines</t>
+          <t>Bacolod_Philippines</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -5525,20 +5525,20 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B137">
         <v>7</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Zamboanga_Philippines</t>
+          <t>Iloilo_Philippines</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -5563,20 +5563,20 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B138">
         <v>7</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Imus_Philippines</t>
+          <t>Tagbilaran_Philippines</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -5601,20 +5601,20 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B139">
         <v>7</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Santa_Rosa_Philippines</t>
+          <t>Misasmis_Oriental_Philippines</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -5639,20 +5639,20 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B140">
         <v>7</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Calamba_Philippines</t>
+          <t>Davao_Philippines</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -5677,20 +5677,20 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B141">
         <v>7</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Monte_Grande_Argentina</t>
+          <t>Zamboanga_Philippines</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -5715,20 +5715,20 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B142">
         <v>7</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Maracaibo_Venezuela</t>
+          <t>Imus_Philippines</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -5753,20 +5753,20 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B143">
         <v>7</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Valencia_Venezuela</t>
+          <t>Santa_Rosa_Philippines</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -5791,20 +5791,20 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B144">
         <v>7</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Antimano_Venezuela</t>
+          <t>Calamba_Philippines</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -5829,20 +5829,20 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B145">
         <v>7</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Barcelona_Venezuela</t>
+          <t>Monte_Grande_Argentina</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -5867,20 +5867,20 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B146">
         <v>7</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>San_Jose_Costa_Rica</t>
+          <t>Maracaibo_Venezuela</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -5905,20 +5905,20 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B147">
         <v>7</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Coronado_Costa_Rica</t>
+          <t>Valencia_Venezuela</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -5943,20 +5943,20 @@
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B148">
         <v>7</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Panama_City_Panama</t>
+          <t>Antimano_Venezuela</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -5981,168 +5981,168 @@
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>All locations</t>
+          <t>Barcelona_Venezuela</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>250</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Clean Room Manufacturing, R&amp;D</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B150">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>All locations</t>
+          <t>San_Jose_Costa_Rica</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>250</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Clean Room Manufacturing, R&amp;D</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B151">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>All locations</t>
+          <t>Coronado_Costa_Rica</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>250</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Clean Room Manufacturing, R&amp;D</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B152">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>All locations</t>
+          <t>Panama_City_Panama</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>250</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Clean Room Manufacturing, R&amp;D</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B153">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -6171,16 +6171,16 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B154">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -6209,16 +6209,16 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>1519750212</v>
+        <v>1519841239</v>
       </c>
       <c r="B155">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
@@ -6247,210 +6247,210 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Tue_Feb_27_11:50:12_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>1519750365</v>
+        <v>1519841239</v>
       </c>
       <c r="B156">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t xml:space="preserve"> All locations </t>
+          <t>All locations</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Manufacturing </t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tue_Feb_27_11:52:45_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>1519750453</v>
+        <v>1519841239</v>
       </c>
       <c r="B157">
         <v>5</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> All locations </t>
+          <t>All locations</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Packaged Foods </t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tue_Feb_27_11:54:13_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>1519752069</v>
+        <v>1519841239</v>
       </c>
       <c r="B158">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> All locations </t>
+          <t>All locations</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Beverage </t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tue_Feb_27_12:21:09_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>1519752218</v>
+        <v>1519841239</v>
       </c>
       <c r="B159">
         <v>7</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> All locations </t>
+          <t>All locations</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Packaged Foods </t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t>-</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tue_Feb_27_12:23:38_EST_2018</t>
+          <t>Wed_Feb_28_13:07:19_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>1519752677</v>
+        <v>1519841853</v>
       </c>
       <c r="B160">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> All locations </t>
+          <t xml:space="preserve"> Boise </t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Beverage </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> 250 </t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> 100 </t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tue_Feb_27_12:31:17_EST_2018</t>
+          <t xml:space="preserve"> Wed_Feb_28_13:17:33_EST_2018</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>1519753183</v>
+        <v>1519843928</v>
       </c>
       <c r="B161">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Stanley_Plaza </t>
+          <t xml:space="preserve"> Boise </t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -6465,7 +6465,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 999 </t>
+          <t xml:space="preserve"> 100 </t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
@@ -6475,83 +6475,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tue_Feb_27_12:39:43_EST_2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162">
-        <v>1519831270</v>
-      </c>
-      <c r="B162">
-        <v>7</v>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Maracaibo_Venezuela </t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 250 </t>
-        </is>
-      </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 100 </t>
-        </is>
-      </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Clean Room Manufacturing, R&amp;D </t>
-        </is>
-      </c>
-      <c r="H162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Wed_Feb_28_10:21:10_EST_2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163">
-        <v>1519831399</v>
-      </c>
-      <c r="B163">
-        <v>7</v>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Campo_Grande_Brazil </t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 250 </t>
-        </is>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 100 </t>
-        </is>
-      </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Fabrication/Assembly </t>
-        </is>
-      </c>
-      <c r="H163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Wed_Feb_28_10:23:19_EST_2018</t>
+          <t xml:space="preserve"> Wed_Feb_28_13:52:08_EST_2018</t>
         </is>
       </c>
     </row>

</xml_diff>